<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min Add version history
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
   <si>
     <t>Version</t>
   </si>
@@ -933,6 +933,12 @@
   </si>
   <si>
     <t>All item add condition: VID1, VID0(Support I2C I/O and Function Generator)</t>
+  </si>
+  <si>
+    <t>Add condition: Spec Cursor ON, Spec Vout Max, Spec Vout Min</t>
+  </si>
+  <si>
+    <t>7, 10, 16, 17</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2260,6 +2266,18 @@
       <c r="E97" s="11"/>
       <c r="F97" s="11" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C98" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index Add version history
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="206">
   <si>
     <t>Version</t>
   </si>
@@ -939,6 +939,12 @@
   </si>
   <si>
     <t>7, 10, 16, 17</t>
+  </si>
+  <si>
+    <t>Delete condition: Index</t>
+  </si>
+  <si>
+    <t>1~16</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2278,6 +2284,18 @@
       <c r="E98" s="11"/>
       <c r="F98" s="11" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C99" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index Type C Item 2~12 add condition: Cx_Offset (x = 1 to 8) Add version history
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="208">
   <si>
     <t>Version</t>
   </si>
@@ -945,6 +945,12 @@
   </si>
   <si>
     <t>1~16</t>
+  </si>
+  <si>
+    <t>2~12</t>
+  </si>
+  <si>
+    <t>Add condition: Cx_Offset (x = 1 to 8)</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99:F99"/>
+      <selection activeCell="C100" sqref="C100:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2296,6 +2302,18 @@
       <c r="E99" s="11"/>
       <c r="F99" s="11" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C100" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index Type C Item 2~12 add condition: Cx_Offset (x = 1 to 8)
Check the column name and number before load the condition file
Add version history
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="209">
   <si>
     <t>Version</t>
   </si>
@@ -951,6 +951,9 @@
   </si>
   <si>
     <t>Add condition: Cx_Offset (x = 1 to 8)</t>
+  </si>
+  <si>
+    <t>Check the column name and number before load the condition file</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100:F100"/>
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2314,6 +2317,16 @@
       <c r="E100" s="11"/>
       <c r="F100" s="11" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="10"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index COT Item 1~15, 17 Add result: VID1, VID0 Type C Item 2~12 add condition: Cx_Offset (x = 1 to 8)
Check the column name and number before load the condition file
Add version history
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="211">
   <si>
     <t>Version</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>Check the column name and number before load the condition file</t>
+  </si>
+  <si>
+    <t>Add result: VID1, VID0</t>
+  </si>
+  <si>
+    <t>1~15, 17</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2327,6 +2333,18 @@
       <c r="E101" s="11"/>
       <c r="F101" s="11" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C102" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index COT Item 1~15, 17 Add result: VID1, VID0 Type C Item 2~12 add condition: Cx_Offset (x = 1 to 8) COT Item 17 delay 1s every count COT Item 17 Add condition: Max Current
Check the column name and number before load the condition file
Save, Save as, Load file can be use other path
Send the test report to email
Add New condition file pushbutton
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="214">
   <si>
     <t>Version</t>
   </si>
@@ -963,6 +963,14 @@
   </si>
   <si>
     <t>Add temp result</t>
+  </si>
+  <si>
+    <t>Add condition: Max Current</t>
+  </si>
+  <si>
+    <t>Add function: 
+Save, Save as, Load file can be use other path
+Send the test report to email</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1052,6 +1060,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1333,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2281,72 +2295,72 @@
       <c r="B97" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="C97" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D97" s="10" t="s">
+      <c r="C97" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11" t="s">
+      <c r="E97" s="9"/>
+      <c r="F97" s="9" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C98" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D98" s="10" t="s">
+      <c r="C98" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11" t="s">
+      <c r="E98" s="9"/>
+      <c r="F98" s="9" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C99" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D99" s="10" t="s">
+      <c r="C99" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11" t="s">
+      <c r="E99" s="9"/>
+      <c r="F99" s="9" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C100" s="10" t="s">
+      <c r="C100" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D100" s="10" t="s">
+      <c r="D100" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11" t="s">
+      <c r="E100" s="9"/>
+      <c r="F100" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="10" t="s">
+      <c r="C101" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D101" s="10"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11" t="s">
+      <c r="D101" s="12"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C102" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102" s="10" t="s">
+      <c r="C102" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11" t="s">
+      <c r="E102" s="9"/>
+      <c r="F102" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2358,6 +2372,28 @@
       <c r="E103" s="11"/>
       <c r="F103" s="11" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C104" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="10">
+        <v>17</v>
+      </c>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C105" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="10"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="13" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.0 COT All Item add condition: VID1, VID0 COT Item 7, 10, 16, 17 add condition: Spec_Cursor_ON, Spec_Vout_Max, Spec_Vout_Min COT Item 1~16 delete condition: Index COT Item 1~15, 17 Add result: VID1, VID0 Type C Item 2~12 add condition: Cx_Offset (x = 1 to 8) COT Item 17 delay 1s every count COT Item 17 Add condition: Max Current COT Item 7, 10, 16, 17 Result add: Font will be changed if data over spec
Check the column name and number before load the condition file
Save, Save as, Load file can be use other path
Send the test report to email
Add New condition file pushbutton
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="215">
   <si>
     <t>Version</t>
   </si>
@@ -971,6 +971,9 @@
     <t>Add function: 
 Save, Save as, Load file can be use other path
 Send the test report to email</t>
+  </si>
+  <si>
+    <t>Result add: Font will be changed if data over spec</t>
   </si>
 </sst>
 </file>
@@ -1347,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2394,6 +2397,18 @@
       <c r="E105" s="11"/>
       <c r="F105" s="13" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C106" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.2 Bug fixed: Send email
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.0\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.2\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="222">
   <si>
     <t>Version</t>
   </si>
@@ -981,6 +981,27 @@
   </si>
   <si>
     <t>Add an information window of email before starting the test.</t>
+  </si>
+  <si>
+    <t>v0.5.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instrument control - oscilloscope
+User can use "Ctrl+C" to copy image.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.5.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug fixed: Send email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1043,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,9 +1102,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1364,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2308,8 +2330,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="97" spans="2:6">
-      <c r="B97" s="10" t="s">
+    <row r="97" spans="1:7" s="14" customFormat="1">
+      <c r="A97" s="13"/>
+      <c r="B97" s="12" t="s">
         <v>200</v>
       </c>
       <c r="C97" s="12" t="s">
@@ -2322,8 +2345,11 @@
       <c r="F97" s="9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="98" spans="2:6">
+      <c r="G97" s="9"/>
+    </row>
+    <row r="98" spans="1:7" s="14" customFormat="1">
+      <c r="A98" s="13"/>
+      <c r="B98" s="12"/>
       <c r="C98" s="12" t="s">
         <v>12</v>
       </c>
@@ -2334,8 +2360,11 @@
       <c r="F98" s="9" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="99" spans="2:6">
+      <c r="G98" s="9"/>
+    </row>
+    <row r="99" spans="1:7" s="14" customFormat="1">
+      <c r="A99" s="13"/>
+      <c r="B99" s="12"/>
       <c r="C99" s="12" t="s">
         <v>12</v>
       </c>
@@ -2346,8 +2375,11 @@
       <c r="F99" s="9" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="100" spans="2:6">
+      <c r="G99" s="9"/>
+    </row>
+    <row r="100" spans="1:7" s="14" customFormat="1">
+      <c r="A100" s="13"/>
+      <c r="B100" s="12"/>
       <c r="C100" s="12" t="s">
         <v>68</v>
       </c>
@@ -2358,8 +2390,11 @@
       <c r="F100" s="9" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="101" spans="2:6">
+      <c r="G100" s="9"/>
+    </row>
+    <row r="101" spans="1:7" s="14" customFormat="1">
+      <c r="A101" s="13"/>
+      <c r="B101" s="12"/>
       <c r="C101" s="12" t="s">
         <v>14</v>
       </c>
@@ -2368,8 +2403,11 @@
       <c r="F101" s="9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="102" spans="2:6">
+      <c r="G101" s="9"/>
+    </row>
+    <row r="102" spans="1:7" s="14" customFormat="1">
+      <c r="A102" s="13"/>
+      <c r="B102" s="12"/>
       <c r="C102" s="12" t="s">
         <v>12</v>
       </c>
@@ -2380,59 +2418,99 @@
       <c r="F102" s="9" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="103" spans="2:6">
-      <c r="C103" s="10" t="s">
+      <c r="G102" s="9"/>
+    </row>
+    <row r="103" spans="1:7" s="14" customFormat="1">
+      <c r="A103" s="13"/>
+      <c r="B103" s="12"/>
+      <c r="C103" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D103" s="10"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11" t="s">
+      <c r="D103" s="12"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="104" spans="2:6">
-      <c r="C104" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D104" s="10">
+      <c r="G103" s="9"/>
+    </row>
+    <row r="104" spans="1:7" s="14" customFormat="1">
+      <c r="A104" s="13"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="12">
         <v>17</v>
       </c>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11" t="s">
+      <c r="E104" s="9"/>
+      <c r="F104" s="9" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="105" spans="2:6" ht="47.25">
-      <c r="C105" s="10" t="s">
+      <c r="G104" s="9"/>
+    </row>
+    <row r="105" spans="1:7" s="14" customFormat="1" ht="47.25">
+      <c r="A105" s="13"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="13" t="s">
+      <c r="D105" s="12"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="8" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="106" spans="2:6">
-      <c r="C106" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="10" t="s">
+      <c r="G105" s="9"/>
+    </row>
+    <row r="106" spans="1:7" s="14" customFormat="1">
+      <c r="A106" s="13"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11" t="s">
+      <c r="E106" s="9"/>
+      <c r="F106" s="9" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="107" spans="2:6">
-      <c r="C107" s="10" t="s">
+      <c r="G106" s="9"/>
+    </row>
+    <row r="107" spans="1:7" s="14" customFormat="1">
+      <c r="A107" s="13"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="D107" s="10"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11" t="s">
+      <c r="D107" s="12"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9" t="s">
         <v>216</v>
+      </c>
+      <c r="G107" s="9"/>
+    </row>
+    <row r="108" spans="1:7" ht="31.5">
+      <c r="B108" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="B109" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D109" s="10"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.3 Modify jitter formula
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.2\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.3\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="225">
   <si>
     <t>Version</t>
   </si>
@@ -1001,6 +1001,18 @@
   </si>
   <si>
     <t>Bug fixed: Send email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.5.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify jitter formula</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1386,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2501,16 +2513,31 @@
       </c>
     </row>
     <row r="109" spans="1:7">
-      <c r="B109" s="10" t="s">
+      <c r="B109" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C109" s="10" t="s">
+      <c r="C109" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="D109" s="10"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11" t="s">
+      <c r="D109" s="12"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="B110" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D110" s="10">
+        <v>12</v>
+      </c>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.3 Modify jitter formula Add measurement result minimum limit: Ton 10ns, Toff 250ns
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="226">
   <si>
     <t>Version</t>
   </si>
@@ -1013,6 +1013,10 @@
   </si>
   <si>
     <t>Modify jitter formula</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Ton limit min: 10ns, Toff limit min: 250ns</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1398,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2526,6 +2530,7 @@
       </c>
     </row>
     <row r="110" spans="1:7">
+      <c r="A110" s="13"/>
       <c r="B110" s="10" t="s">
         <v>222</v>
       </c>
@@ -2538,6 +2543,16 @@
       <c r="E110" s="11"/>
       <c r="F110" s="11" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="13"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.3 Modify jitter formula Add measurement result minimum limit: Ton 10ns, Toff 250ns Ch3 can be set the position manually
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="228">
   <si>
     <t>Version</t>
   </si>
@@ -1017,6 +1017,14 @@
   </si>
   <si>
     <t>Add Ton limit min: 10ns, Toff limit min: 250ns</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch3 can be set the position manually</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1402,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:A111"/>
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2553,6 +2561,19 @@
       <c r="E111" s="11"/>
       <c r="F111" s="11" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="B112" s="10"/>
+      <c r="C112" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D112" s="10">
+        <v>7</v>
+      </c>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.3 COT 12 Modify jitter formula Add measurement result minimum limit: Ton 10ns, Toff 250ns Lx channel add auto scale
COT 7
Ch3 can be set the position manually
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="229">
   <si>
     <t>Version</t>
   </si>
@@ -1025,6 +1025,10 @@
   </si>
   <si>
     <t>Ch3 can be set the position manually</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lx channel add auto scale</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1410,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2564,15 +2568,25 @@
       </c>
     </row>
     <row r="112" spans="1:7">
+      <c r="A112" s="13"/>
       <c r="B112" s="10"/>
-      <c r="C112" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" s="10">
-        <v>7</v>
-      </c>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
       <c r="E112" s="11"/>
       <c r="F112" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6">
+      <c r="B113" s="10"/>
+      <c r="C113" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D113" s="10">
+        <v>7</v>
+      </c>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto_Test_v0.5.4 Add DC load Model: Chroma_63630_80_60, Chroma_63640_80_80 Add current range
COT 1,2,3,4,5,6,8,9,12,13,15,16,17 Auto select mode CCL or CCM or CCH
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.3\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.4\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="234">
   <si>
     <t>Version</t>
   </si>
@@ -1029,6 +1029,25 @@
   </si>
   <si>
     <t>Lx channel add auto scale</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.5.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,8,9,12,13,15,16,17</t>
+  </si>
+  <si>
+    <t>Mode: CCH</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto select mode CCL or CCM or CCH</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1414,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2543,51 +2562,68 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="13"/>
-      <c r="B110" s="10" t="s">
+      <c r="B110" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="C110" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D110" s="10">
-        <v>12</v>
-      </c>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11" t="s">
+      <c r="D110" s="12">
+        <v>12</v>
+      </c>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="13"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11" t="s">
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="13"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11" t="s">
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="113" spans="2:6">
-      <c r="B113" s="10"/>
-      <c r="C113" s="10" t="s">
+      <c r="B113" s="12"/>
+      <c r="C113" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D113" s="12">
         <v>7</v>
       </c>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11" t="s">
+      <c r="E113" s="9"/>
+      <c r="F113" s="9" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.5 COT-8 Measure time of DAQ is maximum -> User can set the measure time of DAQ by burn in time Library	Load_Meter -> Add model: Chroma_63630_80_60
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.4\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.5\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="241">
   <si>
     <t>Version</t>
   </si>
@@ -1048,6 +1048,34 @@
   </si>
   <si>
     <t>Auto select mode CCL or CCM or CCH</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.5.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User can set the measure time of DAQ by burn in time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Measure time of DAQ is maximum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Library</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add model: Chroma_63630_80_60</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load_Meter</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1433,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2610,20 +2638,49 @@
       </c>
     </row>
     <row r="114" spans="2:6">
-      <c r="B114" s="10" t="s">
+      <c r="B114" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="C114" s="10" t="s">
+      <c r="C114" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="D114" s="10" t="s">
+      <c r="D114" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="E114" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="F114" s="9" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6">
+      <c r="B115" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D115" s="10">
+        <v>8</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="C116" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D116" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.5.5 COT-8 Measure time of DAQ is maximum -> User can set the measure time of DAQ by burn in time Library	Load_Meter -> Users can select the same instrument as DC Load.
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -1071,11 +1071,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Add model: Chroma_63630_80_60</t>
+    <t>Load_Meter</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Load_Meter</t>
+    <t>Users can select the same instrument as DC Load.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2676,11 +2676,11 @@
         <v>238</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E116" s="11"/>
       <c r="F116" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other 1, 2 Add IV curve auto test
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.5.5\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.6.0\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="250">
   <si>
     <t>Version</t>
   </si>
@@ -1096,6 +1096,22 @@
   </si>
   <si>
     <t>Add Instrument_Shut_Down function</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.6.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add IV curve auto test</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1481,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F119" sqref="C119:F119"/>
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2644,7 +2660,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="113" spans="2:6">
+    <row r="113" spans="1:7">
       <c r="B113" s="12"/>
       <c r="C113" s="12" t="s">
         <v>226</v>
@@ -2657,7 +2673,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="2:6">
+    <row r="114" spans="1:7">
       <c r="B114" s="12" t="s">
         <v>229</v>
       </c>
@@ -2674,66 +2690,95 @@
         <v>233</v>
       </c>
     </row>
-    <row r="115" spans="2:6">
-      <c r="B115" s="10" t="s">
+    <row r="115" spans="1:7" s="14" customFormat="1">
+      <c r="A115" s="13"/>
+      <c r="B115" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="C115" s="10" t="s">
+      <c r="C115" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="D115" s="10">
+      <c r="D115" s="12">
         <v>8</v>
       </c>
-      <c r="E115" s="11" t="s">
+      <c r="E115" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="F115" s="11" t="s">
+      <c r="F115" s="9" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="116" spans="2:6">
-      <c r="C116" s="10" t="s">
+      <c r="G115" s="9"/>
+    </row>
+    <row r="116" spans="1:7" s="14" customFormat="1">
+      <c r="A116" s="13"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="D116" s="10" t="s">
+      <c r="D116" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11" t="s">
+      <c r="E116" s="9"/>
+      <c r="F116" s="9" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="117" spans="2:6">
-      <c r="C117" s="10" t="s">
+      <c r="G116" s="9"/>
+    </row>
+    <row r="117" spans="1:7" s="14" customFormat="1">
+      <c r="A117" s="13"/>
+      <c r="B117" s="12"/>
+      <c r="C117" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D117" s="10"/>
-      <c r="E117" s="11" t="s">
+      <c r="D117" s="12"/>
+      <c r="E117" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F117" s="11" t="s">
+      <c r="F117" s="9" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="118" spans="2:6">
-      <c r="C118" s="10" t="s">
+      <c r="G117" s="9"/>
+    </row>
+    <row r="118" spans="1:7" s="14" customFormat="1">
+      <c r="A118" s="13"/>
+      <c r="B118" s="12"/>
+      <c r="C118" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="D118" s="10">
+      <c r="D118" s="12">
         <v>8</v>
       </c>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11" t="s">
+      <c r="E118" s="9"/>
+      <c r="F118" s="9" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="119" spans="2:6">
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11" t="s">
+      <c r="G118" s="9"/>
+    </row>
+    <row r="119" spans="1:7" s="14" customFormat="1">
+      <c r="A119" s="13"/>
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9" t="s">
         <v>245</v>
       </c>
+      <c r="G119" s="9"/>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="B120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F120" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other	1, 2	Add IV curve auto test 			Update oscilloscope screen tool COT	1		Add measurement 7: Vout to PG delay COT	1	Delay of enable control is always closed.	Fix the bug
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="256">
   <si>
     <t>Version</t>
   </si>
@@ -1112,6 +1112,30 @@
   </si>
   <si>
     <t>Add IV curve auto test</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update oscilloscope screen tool</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add measurement 7: Vout to PG delay</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix the bug</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delay of enable control is always closed.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1175,7 +1199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1217,6 +1241,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1497,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2766,6 +2793,7 @@
       <c r="G119" s="9"/>
     </row>
     <row r="120" spans="1:7">
+      <c r="A120" s="15"/>
       <c r="B120" s="10" t="s">
         <v>246</v>
       </c>
@@ -2779,6 +2807,46 @@
         <v>249</v>
       </c>
       <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="15"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="15"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D122" s="10">
+        <v>1</v>
+      </c>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="15"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D123" s="10">
+        <v>1</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other	1, 2	Add IV curve auto test 			Update oscilloscope screen tool COT	1		Add measurement 7: Vout to PG delay COT	1	Delay of enable control is always closed.	Fix the bug All			Source meter: Update voltage and current on the instrument once
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="258">
   <si>
     <t>Version</t>
   </si>
@@ -1136,6 +1136,14 @@
   </si>
   <si>
     <t>Delay of enable control is always closed.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source meter: Update voltage and current on the instrument once</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1524,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+      <selection activeCell="F124" sqref="A124:F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2846,6 +2854,18 @@
       </c>
       <c r="F123" s="11" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="15"/>
+      <c r="B124" s="10"/>
+      <c r="C124" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D124" s="10"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="11" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other	1, 2	Add IV curve auto test 			Update oscilloscope screen tool COT	1		Add measurement 7: Vout to PG delay COT	1	Delay of enable control is always closed.	Fix the bug All			Source meter: Update voltage and current on the instrument once COT	All		Turn off all instrument before start to test.
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="261">
   <si>
     <t>Version</t>
   </si>
@@ -1144,6 +1144,18 @@
   </si>
   <si>
     <t>Source meter: Update voltage and current on the instrument once</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn off all instrument before start to test.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1532,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F124" sqref="A124:F124"/>
+      <selection activeCell="F125" sqref="A125:F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2866,6 +2878,20 @@
       <c r="E124" s="11"/>
       <c r="F124" s="11" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="15"/>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other	1, 2	Add IV curve auto test 			Update oscilloscope screen tool COT	1		Add measurement 7: Vout to PG delay COT	1	Delay of enable control is always closed.	Fix the bug All			Source meter: Update voltage and current on the instrument once COT	All		Turn off all instrument before start to test. COT	All	Source meter: sense current range is set auto	Source meter: sense current range is set 0.1
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="265">
   <si>
     <t>Version</t>
   </si>
@@ -1156,6 +1156,22 @@
   </si>
   <si>
     <t>Turn off all instrument before start to test.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source meter: sense current range is set 0.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source meter: sense current range is set auto</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1544,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F125" sqref="A125:F125"/>
+      <selection activeCell="F126" sqref="A126:F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2892,6 +2908,22 @@
       <c r="E125" s="11"/>
       <c r="F125" s="11" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="15"/>
+      <c r="B126" s="10"/>
+      <c r="C126" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D126" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.6.0 Other	1, 2	Add IV curve auto test 			Update oscilloscope screen tool COT	1		Add measurement 7: Vout to PG delay COT	1	Delay of enable control is always closed.	Fix the bug All			Source meter: Update voltage and current on the instrument once COT	All		Turn off all instrument before start to test. COT	All	Source meter: sense current range is set auto	Source meter: sense current range is set 1 COT	1, 2, 3, 4, 5, 6, 7, 16		Add checkbox: Measure_steady_data_checkBox 					Users can measure steady data or not after capturing the waveform. COT	9		Add 1s delay before Enable control on
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="269">
   <si>
     <t>Version</t>
   </si>
@@ -1172,6 +1172,23 @@
   </si>
   <si>
     <t>Source meter: sense current range is set auto</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add checkbox: Measure_steady_data_checkBox
+Users can measure steady data or not after capturing the waveform.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add 1s delay before Enable control on</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1235,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1279,6 +1296,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,17 +1580,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F126" sqref="A126:F126"/>
+      <selection activeCell="A127" sqref="A127:F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="10.75" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.125" style="1"/>
-    <col min="4" max="4" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73" style="3" customWidth="1"/>
     <col min="6" max="6" width="74.875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.25" style="3" bestFit="1" customWidth="1"/>
@@ -2924,6 +2944,34 @@
       </c>
       <c r="F126" s="11" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="31.5">
+      <c r="A127" s="15"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E127" s="11"/>
+      <c r="F127" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="15"/>
+      <c r="B128" s="10"/>
+      <c r="C128" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D128" s="10">
+        <v>9</v>
+      </c>
+      <c r="E128" s="11"/>
+      <c r="F128" s="11" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.7.0.exe SMM	1, 2		Add measurement, optimize COT	1~9		Optimize response and report
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.6.0\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.7.0\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="276">
   <si>
     <t>Version</t>
   </si>
@@ -1189,6 +1189,34 @@
   </si>
   <si>
     <t>Add 1s delay before Enable control on</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0.7.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add measurement, optimize</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimize response and report</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1252,7 +1280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1296,9 +1324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1580,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:F128"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2849,129 +2874,159 @@
       <c r="G119" s="9"/>
     </row>
     <row r="120" spans="1:7">
-      <c r="A120" s="15"/>
-      <c r="B120" s="10" t="s">
+      <c r="A120" s="13"/>
+      <c r="B120" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C120" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D120" s="10" t="s">
+      <c r="D120" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="E120" s="11" t="s">
+      <c r="E120" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="F120" s="11"/>
+      <c r="F120" s="9"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="A121" s="15"/>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11" t="s">
+      <c r="A121" s="13"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:7">
-      <c r="A122" s="15"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10" t="s">
+      <c r="A122" s="13"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="D122" s="10">
+      <c r="D122" s="12">
         <v>1</v>
       </c>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11" t="s">
+      <c r="E122" s="9"/>
+      <c r="F122" s="9" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="123" spans="1:7">
-      <c r="A123" s="15"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="10" t="s">
+      <c r="A123" s="13"/>
+      <c r="B123" s="12"/>
+      <c r="C123" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="D123" s="10">
+      <c r="D123" s="12">
         <v>1</v>
       </c>
-      <c r="E123" s="11" t="s">
+      <c r="E123" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F123" s="11" t="s">
+      <c r="F123" s="9" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="124" spans="1:7">
-      <c r="A124" s="15"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10" t="s">
+      <c r="A124" s="13"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D124" s="10"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11" t="s">
+      <c r="D124" s="12"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" s="15"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10" t="s">
+      <c r="A125" s="13"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D125" s="10" t="s">
+      <c r="D125" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11" t="s">
+      <c r="E125" s="9"/>
+      <c r="F125" s="9" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:7">
-      <c r="A126" s="15"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10" t="s">
+      <c r="A126" s="13"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="D126" s="10" t="s">
+      <c r="D126" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E126" s="11" t="s">
+      <c r="E126" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="F126" s="11" t="s">
+      <c r="F126" s="9" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="31.5">
-      <c r="A127" s="15"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10" t="s">
+      <c r="A127" s="13"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="D127" s="10" t="s">
+      <c r="D127" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="E127" s="11"/>
-      <c r="F127" s="16" t="s">
+      <c r="E127" s="9"/>
+      <c r="F127" s="8" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="128" spans="1:7">
-      <c r="A128" s="15"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10" t="s">
+      <c r="A128" s="13"/>
+      <c r="B128" s="12"/>
+      <c r="C128" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="D128" s="10">
+      <c r="D128" s="12">
         <v>9</v>
       </c>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11" t="s">
+      <c r="E128" s="9"/>
+      <c r="F128" s="9" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="15"/>
+      <c r="B129" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="15"/>
+      <c r="B130" s="10"/>
+      <c r="C130" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.7.0.exe SMM	1, 2		Add measurement, optimize COT	1~9		Optimize response and report COT	All	Vcc current limit: 0.35A	Vcc current limit: 0.5A
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="279">
   <si>
     <t>Version</t>
   </si>
@@ -1217,6 +1217,18 @@
   </si>
   <si>
     <t>Optimize response and report</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc current limit: 0.5A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc current limit: 0.35A</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1605,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+      <selection activeCell="F131" sqref="A131:F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3027,6 +3039,22 @@
       <c r="E130" s="11"/>
       <c r="F130" s="11" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="15"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F131" s="11" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.7.0.exe SMM	1, 2		Add measurement, optimize COT	1~9		Optimize response and report COT	All	Vcc current limit: 0.35A	Vcc current limit: 0.5A COT	1~8		Fix bugs
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="282">
   <si>
     <t>Version</t>
   </si>
@@ -1229,6 +1229,18 @@
   </si>
   <si>
     <t>Vcc current limit: 0.35A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>COT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix bugs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~8</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1617,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="F131" sqref="A131:F131"/>
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3045,7 +3057,7 @@
       <c r="A131" s="15"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>276</v>
@@ -3055,6 +3067,20 @@
       </c>
       <c r="F131" s="11" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="15"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D132" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto_Test_v0.7.1.exe SMM	1, 2		Add measurement, optimize COT	1~9		Optimize response and report COT	All	Vcc current limit: 0.35A	Vcc current limit: 0.5A COT	1~8		Fix bugs COT	18		Add new test item: Item_18_Iout_Sweep_For_PG_Drop_Test
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="283">
   <si>
     <t>Version</t>
   </si>
@@ -1243,6 +1243,9 @@
     <t>1~8</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Add new test item: Item_18_Iout_Sweep_For_PG_Drop_Test</t>
+  </si>
 </sst>
 </file>
 
@@ -1252,7 +1255,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1272,7 +1275,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1351,7 +1354,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1367,7 +1370,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1629,20 +1632,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="F133" sqref="A133:F133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" style="1"/>
-    <col min="4" max="4" width="27.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73" style="3" customWidth="1"/>
-    <col min="6" max="6" width="74.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2038,7 +2041,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="3:6" ht="31.5">
+    <row r="41" spans="3:6" ht="47.25">
       <c r="E41" s="2" t="s">
         <v>87</v>
       </c>
@@ -3081,6 +3084,20 @@
       <c r="E132" s="11"/>
       <c r="F132" s="11" t="s">
         <v>280</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="15"/>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="10">
+        <v>18</v>
+      </c>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3098,13 +3115,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3222,13 +3239,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3317,13 +3334,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3419,13 +3436,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="52.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3510,13 +3527,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.25" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3536,7 +3553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="33">
+    <row r="2" spans="1:6" ht="30">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -3564,14 +3581,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.25" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3591,7 +3608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="49.5">
+    <row r="2" spans="1:6" ht="45">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -3617,7 +3634,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto_Test_v0.8.0 COT	16	measure error	fix bugs Library	Chamber		Add new library Instrument Control			Add Chamber
</commit_message>
<xml_diff>
--- a/Auto test GUI Version History.xlsx
+++ b/Auto test GUI Version History.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.7.0\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rex\Auto test GUI v0.8.0\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="289">
   <si>
     <t>Version</t>
   </si>
@@ -1245,6 +1245,24 @@
   </si>
   <si>
     <t>Add new test item: Item_18_Iout_Sweep_For_PG_Drop_Test</t>
+  </si>
+  <si>
+    <t>v0.8.0</t>
+  </si>
+  <si>
+    <t>measure error</t>
+  </si>
+  <si>
+    <t>fix bugs</t>
+  </si>
+  <si>
+    <t>Chamber</t>
+  </si>
+  <si>
+    <t>Add new library</t>
+  </si>
+  <si>
+    <t>Add Chamber</t>
   </si>
 </sst>
 </file>
@@ -1632,16 +1650,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="F133" sqref="A133:F133"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F136" sqref="A135:F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73" style="3" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -3027,77 +3046,121 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="15"/>
-      <c r="B129" s="10" t="s">
+      <c r="A129" s="13"/>
+      <c r="B129" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="C129" s="10" t="s">
+      <c r="C129" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="D129" s="10" t="s">
+      <c r="D129" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="E129" s="11"/>
-      <c r="F129" s="11" t="s">
+      <c r="E129" s="9"/>
+      <c r="F129" s="9" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" s="15"/>
-      <c r="B130" s="10"/>
-      <c r="C130" s="10" t="s">
+      <c r="A130" s="13"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="D130" s="10" t="s">
+      <c r="D130" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11" t="s">
+      <c r="E130" s="9"/>
+      <c r="F130" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="15"/>
-      <c r="B131" s="10"/>
-      <c r="C131" s="10" t="s">
+      <c r="A131" s="13"/>
+      <c r="B131" s="12"/>
+      <c r="C131" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="D131" s="10" t="s">
+      <c r="D131" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E131" s="11" t="s">
+      <c r="E131" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="F131" s="11" t="s">
+      <c r="F131" s="9" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="15"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="10" t="s">
+      <c r="A132" s="13"/>
+      <c r="B132" s="12"/>
+      <c r="C132" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="D132" s="10" t="s">
+      <c r="D132" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11" t="s">
+      <c r="E132" s="9"/>
+      <c r="F132" s="9" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="133" spans="1:6">
-      <c r="A133" s="15"/>
-      <c r="B133" s="10"/>
-      <c r="C133" s="10" t="s">
+      <c r="A133" s="13"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="10">
+      <c r="D133" s="12">
         <v>18</v>
       </c>
-      <c r="E133" s="11"/>
-      <c r="F133" s="11" t="s">
+      <c r="E133" s="9"/>
+      <c r="F133" s="9" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="15"/>
+      <c r="B134" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C134" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="10">
+        <v>16</v>
+      </c>
+      <c r="E134" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F134" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="15"/>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D135" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="15"/>
+      <c r="B136" s="10"/>
+      <c r="C136" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D136" s="10"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>